<commit_message>
Atualização do backlog e remoção do arquivo MVV na pasta de documentação
</commit_message>
<xml_diff>
--- a/documentação/TI-Aula3-Backlog.xlsx
+++ b/documentação/TI-Aula3-Backlog.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\bandtec\Banco de Dados\projeto2.0\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aluno\Desktop\git\Projeto2.0\documentação\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="76">
   <si>
     <t>Nomes</t>
   </si>
@@ -76,9 +76,6 @@
     <t>RF4</t>
   </si>
   <si>
-    <t>O produto físico será um latão de lixo;</t>
-  </si>
-  <si>
     <t>RF7</t>
   </si>
   <si>
@@ -100,15 +97,9 @@
     <t>RF6</t>
   </si>
   <si>
-    <t>O site deverá posuir página para cadastro;</t>
-  </si>
-  <si>
     <t>RF9</t>
   </si>
   <si>
-    <t>O site deverá posuir campos para login e senha no canto superior da página inicial;</t>
-  </si>
-  <si>
     <t>O site deverá possuir uma página sobre o nosso produto com uma breve explicação de como funciona;</t>
   </si>
   <si>
@@ -127,9 +118,6 @@
     <t>RF13</t>
   </si>
   <si>
-    <t>O site deverá possuir uma página 'fale conosco' onde será possível encontrar informações para contato com a MIT;</t>
-  </si>
-  <si>
     <t>RF14</t>
   </si>
   <si>
@@ -151,9 +139,6 @@
     <t>RF19</t>
   </si>
   <si>
-    <t>desejavel</t>
-  </si>
-  <si>
     <t>RF20</t>
   </si>
   <si>
@@ -190,9 +175,6 @@
     <t>RF31</t>
   </si>
   <si>
-    <t>O produto físico deverá possuir um sensor de presença;</t>
-  </si>
-  <si>
     <t>O banco de dados deverá possuir as entidades que façam atualizações constante e as entidades que não façam atualizações constante;</t>
   </si>
   <si>
@@ -223,10 +205,49 @@
     <t>O sistema deverá ter um sensor de nivel de agua, para monitorar quantidade de resíduos líquidos;</t>
   </si>
   <si>
-    <t>No site o usuário poderá escolher quantas e quais lixeiras ele irá comprar;</t>
-  </si>
-  <si>
     <t xml:space="preserve">O Dashboard deverá mostrar aos usuários informações e estatísticas com base no banco de dados da MIT; </t>
+  </si>
+  <si>
+    <t>O produto físico será uma lata de lixo inteligente;</t>
+  </si>
+  <si>
+    <t>O produto físico deverá possuir três sensores de presença dentro da lixeira e um na entrada da lixeira;</t>
+  </si>
+  <si>
+    <t>O site deverá possuir página para cadastro;</t>
+  </si>
+  <si>
+    <t>O site deverá possuir uma página para login;</t>
+  </si>
+  <si>
+    <t>O site deverá possuir uma campo  "fale conosco" onde será possível encontrar informações para contato com a MIT;</t>
+  </si>
+  <si>
+    <t>Na página do simulador financeiro o usuário poderá escolher quantas e quais lixeiras ele irá alugar;</t>
+  </si>
+  <si>
+    <t>desejável</t>
+  </si>
+  <si>
+    <t>O projeto deverá possuir uma modelagem conceitual sobre o banco de dados;</t>
+  </si>
+  <si>
+    <t>As entidades estabelecidas no modelo conceitual deverá ser implementada no banco de dados Azure;</t>
+  </si>
+  <si>
+    <t>O projeto deverá possuir o script de criação do banco de dados;</t>
+  </si>
+  <si>
+    <t>O projeto deverá possuir Teste Integrado (Arduino+DB) + API local com Node.JS;</t>
+  </si>
+  <si>
+    <t>O projeto deverá ter um diagrama de arquitetura Local (Arduíno);</t>
+  </si>
+  <si>
+    <t>RF32</t>
+  </si>
+  <si>
+    <t>Sprint 1  a dd-mm</t>
   </si>
 </sst>
 </file>
@@ -236,12 +257,19 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="00000000"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -268,7 +296,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -311,6 +339,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -339,24 +379,24 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -366,7 +406,7 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -374,11 +414,32 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -722,8 +783,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -770,27 +831,27 @@
       <c r="E2" s="5">
         <v>1</v>
       </c>
-      <c r="F2" s="13" t="s">
-        <v>12</v>
+      <c r="F2" s="25" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="30" customHeight="1">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="16" t="s">
+      <c r="B3" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="C3" s="20" t="s">
         <v>11</v>
       </c>
       <c r="D3" s="18">
         <v>8</v>
       </c>
-      <c r="E3" s="5">
+      <c r="E3" s="20">
         <v>2</v>
       </c>
-      <c r="F3" s="13" t="s">
+      <c r="F3" s="20" t="s">
         <v>12</v>
       </c>
     </row>
@@ -818,8 +879,8 @@
       <c r="A5" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="16" t="s">
-        <v>18</v>
+      <c r="B5" s="21" t="s">
+        <v>62</v>
       </c>
       <c r="C5" s="9" t="s">
         <v>11</v>
@@ -835,11 +896,11 @@
       </c>
     </row>
     <row r="6" spans="1:6" ht="30" customHeight="1">
-      <c r="A6" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="B6" s="16" t="s">
-        <v>56</v>
+      <c r="A6" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" s="21" t="s">
+        <v>63</v>
       </c>
       <c r="C6" s="9" t="s">
         <v>11</v>
@@ -851,15 +912,15 @@
         <v>5</v>
       </c>
       <c r="F6" s="13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="30">
       <c r="A7" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="B7" s="16" t="s">
-        <v>57</v>
+        <v>24</v>
+      </c>
+      <c r="B7" s="21" t="s">
+        <v>51</v>
       </c>
       <c r="C7" s="9" t="s">
         <v>11</v>
@@ -871,55 +932,55 @@
         <v>6</v>
       </c>
       <c r="F7" s="13" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="30">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="27.75" customHeight="1">
       <c r="A8" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="B8" s="16" t="s">
-        <v>58</v>
+        <v>18</v>
+      </c>
+      <c r="B8" s="21" t="s">
+        <v>71</v>
       </c>
       <c r="C8" s="9" t="s">
         <v>11</v>
       </c>
       <c r="D8" s="9">
-        <v>21</v>
+        <v>5</v>
       </c>
       <c r="E8" s="5">
         <v>7</v>
       </c>
       <c r="F8" s="13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="30" customHeight="1">
-      <c r="A9" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="B9" s="16" t="s">
-        <v>59</v>
+      <c r="A9" s="23" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" s="21" t="s">
+        <v>69</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="D9" s="9">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="E9" s="5">
         <v>8</v>
       </c>
       <c r="F9" s="13" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="30" customHeight="1">
       <c r="A10" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="B10" s="16" t="s">
-        <v>26</v>
+      <c r="B10" s="21" t="s">
+        <v>70</v>
       </c>
       <c r="C10" s="9" t="s">
         <v>11</v>
@@ -931,18 +992,18 @@
         <v>9</v>
       </c>
       <c r="F10" s="13" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="30" customHeight="1">
       <c r="A11" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="B11" s="16" t="s">
-        <v>28</v>
+        <v>20</v>
+      </c>
+      <c r="B11" s="21" t="s">
+        <v>52</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="D11" s="9">
         <v>21</v>
@@ -951,20 +1012,20 @@
         <v>10</v>
       </c>
       <c r="F11" s="13" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="30" customHeight="1">
-      <c r="A12" s="7" t="s">
-        <v>21</v>
+      <c r="A12" s="23" t="s">
+        <v>27</v>
       </c>
       <c r="B12" s="16" t="s">
-        <v>29</v>
+        <v>53</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="D12" s="11">
+        <v>23</v>
+      </c>
+      <c r="D12" s="9">
         <v>8</v>
       </c>
       <c r="E12" s="5">
@@ -976,16 +1037,16 @@
     </row>
     <row r="13" spans="1:6" ht="30" customHeight="1">
       <c r="A13" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="B13" s="16" t="s">
-        <v>60</v>
+        <v>28</v>
+      </c>
+      <c r="B13" s="21" t="s">
+        <v>64</v>
       </c>
       <c r="C13" s="9" t="s">
         <v>11</v>
       </c>
       <c r="D13" s="9">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="E13" s="5">
         <v>12</v>
@@ -994,15 +1055,15 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="30">
+    <row r="14" spans="1:6" ht="30" customHeight="1">
       <c r="A14" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="B14" s="16" t="s">
-        <v>32</v>
+      <c r="B14" s="21" t="s">
+        <v>65</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="D14" s="9">
         <v>21</v>
@@ -1011,41 +1072,41 @@
         <v>13</v>
       </c>
       <c r="F14" s="13" t="s">
-        <v>33</v>
+        <v>12</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="30" customHeight="1">
-      <c r="A15" s="7" t="s">
-        <v>34</v>
+      <c r="A15" s="23" t="s">
+        <v>32</v>
       </c>
       <c r="B15" s="16" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="D15" s="9">
+        <v>11</v>
+      </c>
+      <c r="D15" s="11">
         <v>8</v>
       </c>
       <c r="E15" s="5">
         <v>14</v>
       </c>
       <c r="F15" s="13" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="30" customHeight="1">
-      <c r="A16" s="7" t="s">
-        <v>36</v>
+      <c r="A16" s="23" t="s">
+        <v>34</v>
       </c>
       <c r="B16" s="16" t="s">
-        <v>67</v>
+        <v>54</v>
       </c>
       <c r="C16" s="9" t="s">
         <v>11</v>
       </c>
       <c r="D16" s="9">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="E16" s="5">
         <v>15</v>
@@ -1055,51 +1116,51 @@
       </c>
     </row>
     <row r="17" spans="1:6" ht="30" customHeight="1">
-      <c r="A17" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="B17" s="16" t="s">
-        <v>68</v>
-      </c>
-      <c r="C17" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="D17" s="9">
-        <v>21</v>
-      </c>
-      <c r="E17" s="5">
+      <c r="A17" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="B17" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="C17" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="D17" s="20">
+        <v>21</v>
+      </c>
+      <c r="E17" s="20">
         <v>16</v>
       </c>
-      <c r="F17" s="13" t="s">
-        <v>20</v>
+      <c r="F17" s="20" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="30" customHeight="1">
-      <c r="A18" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="B18" s="16" t="s">
-        <v>37</v>
+      <c r="A18" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="B18" s="21" t="s">
+        <v>66</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="D18" s="9">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="E18" s="5">
         <v>17</v>
       </c>
       <c r="F18" s="13" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="30" customHeight="1">
       <c r="A19" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="B19" s="16" t="s">
-        <v>61</v>
+        <v>37</v>
+      </c>
+      <c r="B19" s="21" t="s">
+        <v>67</v>
       </c>
       <c r="C19" s="9" t="s">
         <v>11</v>
@@ -1111,15 +1172,15 @@
         <v>18</v>
       </c>
       <c r="F19" s="13" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="30" customHeight="1">
       <c r="A20" s="7" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B20" s="16" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C20" s="9" t="s">
         <v>11</v>
@@ -1131,15 +1192,15 @@
         <v>19</v>
       </c>
       <c r="F20" s="13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="30" customHeight="1">
-      <c r="A21" s="7" t="s">
-        <v>42</v>
+      <c r="A21" s="23" t="s">
+        <v>39</v>
       </c>
       <c r="B21" s="16" t="s">
-        <v>63</v>
+        <v>33</v>
       </c>
       <c r="C21" s="9" t="s">
         <v>11</v>
@@ -1151,15 +1212,15 @@
         <v>20</v>
       </c>
       <c r="F21" s="13" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" ht="30">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="28.5" customHeight="1">
       <c r="A22" s="7" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B22" s="16" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="C22" s="9" t="s">
         <v>11</v>
@@ -1171,102 +1232,152 @@
         <v>21</v>
       </c>
       <c r="F22" s="13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="30" customHeight="1">
       <c r="A23" s="7" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B23" s="16" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>43</v>
+        <v>11</v>
       </c>
       <c r="D23" s="9">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="E23" s="5">
         <v>22</v>
       </c>
       <c r="F23" s="13" t="s">
-        <v>33</v>
+        <v>19</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="30" customHeight="1">
-      <c r="A24" s="7" t="s">
-        <v>46</v>
+      <c r="A24" s="23" t="s">
+        <v>42</v>
       </c>
       <c r="B24" s="16" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="C24" s="9" t="s">
-        <v>43</v>
+        <v>11</v>
       </c>
       <c r="D24" s="9">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="E24" s="5">
         <v>23</v>
       </c>
       <c r="F24" s="13" t="s">
-        <v>33</v>
+        <v>19</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="30" customHeight="1">
       <c r="A25" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="B25" s="16"/>
-      <c r="C25" s="9"/>
-      <c r="D25" s="9"/>
-      <c r="E25" s="5"/>
-      <c r="F25" s="13"/>
+        <v>43</v>
+      </c>
+      <c r="B25" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="C25" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="D25" s="9">
+        <v>21</v>
+      </c>
+      <c r="E25" s="5">
+        <v>24</v>
+      </c>
+      <c r="F25" s="13" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="26" spans="1:6" ht="30" customHeight="1">
       <c r="A26" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="B26" s="16"/>
-      <c r="C26" s="9"/>
-      <c r="D26" s="9"/>
-      <c r="E26" s="5"/>
-      <c r="F26" s="13"/>
+        <v>44</v>
+      </c>
+      <c r="B26" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="C26" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="D26" s="9">
+        <v>8</v>
+      </c>
+      <c r="E26" s="5">
+        <v>25</v>
+      </c>
+      <c r="F26" s="13" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="27" spans="1:6" ht="30" customHeight="1">
-      <c r="A27" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="B27" s="16"/>
-      <c r="C27" s="9"/>
-      <c r="D27" s="9"/>
-      <c r="E27" s="5"/>
-      <c r="F27" s="13"/>
+      <c r="A27" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="B27" s="19" t="s">
+        <v>60</v>
+      </c>
+      <c r="C27" s="20" t="s">
+        <v>68</v>
+      </c>
+      <c r="D27" s="20">
+        <v>8</v>
+      </c>
+      <c r="E27" s="20">
+        <v>26</v>
+      </c>
+      <c r="F27" s="20" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="28" spans="1:6" ht="30" customHeight="1">
       <c r="A28" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="B28" s="16"/>
-      <c r="C28" s="9"/>
-      <c r="D28" s="9"/>
-      <c r="E28" s="5"/>
-      <c r="F28" s="13"/>
+        <v>46</v>
+      </c>
+      <c r="B28" s="21" t="s">
+        <v>72</v>
+      </c>
+      <c r="C28" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="D28" s="9">
+        <v>21</v>
+      </c>
+      <c r="E28" s="5">
+        <v>27</v>
+      </c>
+      <c r="F28" s="13" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="29" spans="1:6" ht="30" customHeight="1">
       <c r="A29" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="B29" s="16"/>
-      <c r="C29" s="9"/>
-      <c r="D29" s="9"/>
-      <c r="E29" s="5"/>
-      <c r="F29" s="13"/>
+        <v>47</v>
+      </c>
+      <c r="B29" s="21" t="s">
+        <v>73</v>
+      </c>
+      <c r="C29" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="D29" s="9">
+        <v>21</v>
+      </c>
+      <c r="E29" s="5">
+        <v>28</v>
+      </c>
+      <c r="F29" s="13" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="30" spans="1:6" ht="30" customHeight="1">
-      <c r="A30" s="7" t="s">
-        <v>52</v>
+      <c r="A30" s="23" t="s">
+        <v>48</v>
       </c>
       <c r="B30" s="16"/>
       <c r="C30" s="9"/>
@@ -1276,7 +1387,7 @@
     </row>
     <row r="31" spans="1:6" ht="30" customHeight="1">
       <c r="A31" s="7" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B31" s="16"/>
       <c r="C31" s="9"/>
@@ -1286,7 +1397,7 @@
     </row>
     <row r="32" spans="1:6" ht="30" customHeight="1">
       <c r="A32" s="7" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B32" s="16"/>
       <c r="C32" s="9"/>
@@ -1295,8 +1406,8 @@
       <c r="F32" s="13"/>
     </row>
     <row r="33" spans="1:6" ht="30" customHeight="1">
-      <c r="A33" s="7" t="s">
-        <v>55</v>
+      <c r="A33" s="23" t="s">
+        <v>74</v>
       </c>
       <c r="B33" s="16"/>
       <c r="C33" s="9"/>

</xml_diff>